<commit_message>
added column names to china CSVs
</commit_message>
<xml_diff>
--- a/inst/extdata/gcam-china/NBS_CESY_mappings.xlsx
+++ b/inst/extdata/gcam-china/NBS_CESY_mappings.xlsx
@@ -1,16 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25317"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="21328"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\yarl762\Desktop\GitHub\gcamdata\inst\extdata\gcam-china\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{16C5EC9F-F3AF-486B-9343-D53A54EE94DD}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3940" yWindow="1740" windowWidth="25600" windowHeight="18380" tabRatio="500"/>
+    <workbookView xWindow="10290" yWindow="2040" windowWidth="17295" windowHeight="13485" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="NBS_CESY_process" sheetId="1" r:id="rId1"/>
     <sheet name="NBS_CESY_material" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="140000" concurrentCalc="0"/>
+  <calcPr calcId="140000"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -20,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="131" uniqueCount="98">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="133" uniqueCount="100">
   <si>
     <t>Total Primary Energy Supply</t>
   </si>
@@ -314,12 +320,18 @@
   </si>
   <si>
     <t>industry_feedstocks</t>
+  </si>
+  <si>
+    <t># ----------</t>
+  </si>
+  <si>
+    <t># Column types: cc</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -429,6 +441,14 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -753,308 +773,318 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B42"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:B44"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B19" sqref="B19"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="71" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>94</v>
       </c>
     </row>
-    <row r="2" spans="1:2">
+    <row r="2" spans="1:2" ht="15" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
         <v>80</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B4" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="3" spans="1:2">
-      <c r="A3" t="s">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
         <v>24</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B5" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="4" spans="1:2">
-      <c r="A4" t="s">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="5" spans="1:2">
-      <c r="A5" t="s">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="6" spans="1:2">
-      <c r="A6" t="s">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="7" spans="1:2">
-      <c r="A7" t="s">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="8" spans="1:2">
-      <c r="A8" t="s">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
         <v>29</v>
       </c>
-      <c r="B8" t="s">
+      <c r="B10" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="9" spans="1:2">
-      <c r="A9" t="s">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="10" spans="1:2">
-      <c r="A10" t="s">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
         <v>10</v>
       </c>
-      <c r="B10" t="s">
+      <c r="B12" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="11" spans="1:2">
-      <c r="A11" t="s">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
         <v>18</v>
       </c>
-      <c r="B11" t="s">
+      <c r="B13" t="s">
         <v>84</v>
       </c>
     </row>
-    <row r="12" spans="1:2">
-      <c r="A12" t="s">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
         <v>19</v>
       </c>
-      <c r="B12" t="s">
+      <c r="B14" t="s">
         <v>84</v>
       </c>
     </row>
-    <row r="13" spans="1:2">
-      <c r="A13" t="s">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
         <v>14</v>
       </c>
-      <c r="B13" t="s">
+      <c r="B15" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="14" spans="1:2">
-      <c r="A14" t="s">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
         <v>26</v>
       </c>
-      <c r="B14" t="s">
+      <c r="B16" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="15" spans="1:2">
-      <c r="A15" t="s">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="16" spans="1:2">
-      <c r="A16" t="s">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
         <v>1</v>
       </c>
-      <c r="B16" t="s">
+      <c r="B18" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="17" spans="1:2">
-      <c r="A17" t="s">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
         <v>2</v>
       </c>
-      <c r="B17" t="s">
+      <c r="B19" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="18" spans="1:2">
-      <c r="A18" t="s">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
         <v>3</v>
       </c>
-      <c r="B18" t="s">
+      <c r="B20" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="19" spans="1:2">
-      <c r="A19" t="s">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
         <v>25</v>
       </c>
-      <c r="B19" t="s">
+      <c r="B21" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="20" spans="1:2">
-      <c r="A20" t="s">
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
         <v>28</v>
       </c>
-      <c r="B20" t="s">
+      <c r="B22" t="s">
         <v>97</v>
       </c>
     </row>
-    <row r="21" spans="1:2">
-      <c r="A21" t="s">
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="22" spans="1:2">
-      <c r="A22" t="s">
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="23" spans="1:2">
-      <c r="A23" t="s">
+    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
         <v>27</v>
-      </c>
-      <c r="B23" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="24" spans="1:2">
-      <c r="A24" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="25" spans="1:2">
-      <c r="A25" t="s">
-        <v>23</v>
       </c>
       <c r="B25" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="26" spans="1:2">
+    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>38</v>
-      </c>
-      <c r="B26" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="27" spans="1:2">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>32</v>
+        <v>23</v>
       </c>
       <c r="B27" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="28" spans="1:2">
+    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
+        <v>38</v>
+      </c>
+      <c r="B28" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>32</v>
+      </c>
+      <c r="B29" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
         <v>36</v>
       </c>
-      <c r="B28" t="s">
+      <c r="B30" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="29" spans="1:2">
-      <c r="A29" t="s">
+    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
         <v>17</v>
       </c>
-      <c r="B29" t="s">
+      <c r="B31" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="30" spans="1:2">
-      <c r="A30" t="s">
+    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
         <v>39</v>
       </c>
-      <c r="B30" t="s">
+      <c r="B32" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="31" spans="1:2">
-      <c r="A31" t="s">
+    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="32" spans="1:2">
-      <c r="A32" t="s">
+    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
         <v>33</v>
       </c>
-      <c r="B32" t="s">
+      <c r="B34" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="33" spans="1:2">
-      <c r="A33" t="s">
+    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
         <v>34</v>
       </c>
-      <c r="B33" t="s">
+      <c r="B35" t="s">
         <v>90</v>
       </c>
     </row>
-    <row r="34" spans="1:2">
-      <c r="A34" t="s">
+    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
         <v>35</v>
       </c>
-      <c r="B34" t="s">
+      <c r="B36" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="35" spans="1:2">
-      <c r="A35" t="s">
+    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="36" spans="1:2">
-      <c r="A36" t="s">
+    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="37" spans="1:2">
-      <c r="A37" t="s">
+    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
         <v>13</v>
       </c>
-      <c r="B37" t="s">
+      <c r="B39" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="38" spans="1:2">
-      <c r="A38" t="s">
+    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A40" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="39" spans="1:2">
-      <c r="A39" t="s">
+    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A41" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="40" spans="1:2">
-      <c r="A40" t="s">
+    <row r="42" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A42" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="41" spans="1:2">
-      <c r="A41" t="s">
+    <row r="43" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A43" t="s">
         <v>30</v>
       </c>
-      <c r="B41" t="s">
+      <c r="B43" t="s">
         <v>93</v>
       </c>
     </row>
-    <row r="42" spans="1:2">
-      <c r="A42" t="s">
+    <row r="44" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A44" t="s">
         <v>31</v>
       </c>
-      <c r="B42" t="s">
+      <c r="B44" t="s">
         <v>92</v>
       </c>
     </row>
   </sheetData>
-  <sortState ref="A1:A38">
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A1:A40">
     <sortCondition ref="A1"/>
   </sortState>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -1068,24 +1098,24 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:B35"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="69.83203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="69.875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="2" spans="1:2">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>73</v>
       </c>
@@ -1093,12 +1123,12 @@
         <v>74</v>
       </c>
     </row>
-    <row r="3" spans="1:2">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="4" spans="1:2">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>64</v>
       </c>
@@ -1106,7 +1136,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="5" spans="1:2">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>44</v>
       </c>
@@ -1114,7 +1144,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="6" spans="1:2">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>42</v>
       </c>
@@ -1122,7 +1152,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="7" spans="1:2">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>47</v>
       </c>
@@ -1130,7 +1160,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="8" spans="1:2">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>41</v>
       </c>
@@ -1138,7 +1168,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="9" spans="1:2">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>43</v>
       </c>
@@ -1146,7 +1176,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="10" spans="1:2">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>45</v>
       </c>
@@ -1154,7 +1184,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="11" spans="1:2">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>48</v>
       </c>
@@ -1162,7 +1192,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="12" spans="1:2">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>46</v>
       </c>
@@ -1170,7 +1200,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="13" spans="1:2">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>65</v>
       </c>
@@ -1178,7 +1208,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="14" spans="1:2">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>50</v>
       </c>
@@ -1186,7 +1216,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="15" spans="1:2">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>53</v>
       </c>
@@ -1194,7 +1224,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="16" spans="1:2">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>60</v>
       </c>
@@ -1202,7 +1232,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="17" spans="1:2">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>54</v>
       </c>
@@ -1210,7 +1240,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="18" spans="1:2">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>66</v>
       </c>
@@ -1218,7 +1248,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="19" spans="1:2">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>51</v>
       </c>
@@ -1226,7 +1256,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="20" spans="1:2">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>59</v>
       </c>
@@ -1234,7 +1264,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="21" spans="1:2">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>52</v>
       </c>
@@ -1242,7 +1272,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="22" spans="1:2">
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>55</v>
       </c>
@@ -1250,7 +1280,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="23" spans="1:2">
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>67</v>
       </c>
@@ -1258,7 +1288,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="24" spans="1:2">
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>68</v>
       </c>
@@ -1266,7 +1296,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="25" spans="1:2">
+    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>69</v>
       </c>
@@ -1274,7 +1304,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="26" spans="1:2">
+    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>57</v>
       </c>
@@ -1282,12 +1312,12 @@
         <v>79</v>
       </c>
     </row>
-    <row r="27" spans="1:2">
+    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="28" spans="1:2">
+    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>70</v>
       </c>
@@ -1295,7 +1325,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="29" spans="1:2">
+    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>58</v>
       </c>
@@ -1303,7 +1333,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="30" spans="1:2">
+    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>71</v>
       </c>
@@ -1311,7 +1341,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="31" spans="1:2">
+    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>56</v>
       </c>
@@ -1319,28 +1349,28 @@
         <v>76</v>
       </c>
     </row>
-    <row r="32" spans="1:2">
+    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="33" spans="1:1">
+    <row r="33" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="34" spans="1:1">
+    <row r="34" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="35" spans="1:1">
+    <row r="35" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>49</v>
       </c>
     </row>
   </sheetData>
-  <sortState ref="A1:A23">
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A1:A23">
     <sortCondition ref="A1"/>
   </sortState>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>